<commit_message>
updated Security Requirements Taxonomy (added extended CIA discussion) / updated cybersecurity requirements spreadsheet (removed functional requirements / corrected spelling error)
</commit_message>
<xml_diff>
--- a/distribution/reference_documents/working_material/cybersecurity requirements per taxonomy.xlsx
+++ b/distribution/reference_documents/working_material/cybersecurity requirements per taxonomy.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.wilson/Documents/projects/AVCDL/source/reference_documents/working_material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B301CB-CAD9-BD46-AA2D-9C750771467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107ADBD8-83C0-1A42-8A29-CABC48DE0EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44160" yWindow="1320" windowWidth="31560" windowHeight="30120" xr2:uid="{56895247-3B3D-3147-A316-D5FB82A09ACE}"/>
+    <workbookView xWindow="24660" yWindow="800" windowWidth="23320" windowHeight="28160" activeTab="1" xr2:uid="{56895247-3B3D-3147-A316-D5FB82A09ACE}"/>
   </bookViews>
   <sheets>
     <sheet name="layer-asset-property sort" sheetId="5" r:id="rId1"/>
+    <sheet name="asset-property-layer sort" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="89">
   <si>
     <t>Property</t>
   </si>
@@ -118,9 +119,6 @@
     <t>Privileged access shall be permitted only for singular, specific, time-limited operations.</t>
   </si>
   <si>
-    <t>The system shall contain only secure default privileged accounts, if a privileged account is necessary.</t>
-  </si>
-  <si>
     <t>Memory</t>
   </si>
   <si>
@@ -142,9 +140,6 @@
     <t>Logs shall be stored in encrypted volumes.</t>
   </si>
   <si>
-    <t>Logs shall utilize defined terminology, abbreviations, and acronyms.</t>
-  </si>
-  <si>
     <t>Deviations from standard, normal, or expected conditions shall be detected.</t>
   </si>
   <si>
@@ -265,9 +260,6 @@
     <t>PII data transmission shall be recorded in the audit log.</t>
   </si>
   <si>
-    <t>Cyprtographic material stored in memory shall be validated prior to use.</t>
-  </si>
-  <si>
     <t>Credentials shall be encrypted when transmitted across trust boundaries.</t>
   </si>
   <si>
@@ -305,6 +297,12 @@
   </si>
   <si>
     <t>Cryptographic operations shall use a mechanism that is backed by a hardware root of trust.</t>
+  </si>
+  <si>
+    <t>The system shall contain only secure default privileged accounts if a privileged account is necessary.</t>
+  </si>
+  <si>
+    <t>Cryptographic material stored in memory shall be validated prior to use.</t>
   </si>
 </sst>
 </file>
@@ -714,11 +712,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96C74873-220C-9F48-A83A-36F8D7B5B9A6}">
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:V65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A55" sqref="A55"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,7 +729,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>0</v>
@@ -743,7 +741,7 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -773,7 +771,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>8</v>
@@ -788,13 +786,13 @@
         <v>4</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>12</v>
@@ -809,7 +807,7 @@
         <v>6</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>16</v>
@@ -829,11 +827,11 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -841,32 +839,32 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S3" s="8"/>
       <c r="V3" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -874,20 +872,20 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S4" s="8"/>
       <c r="V4" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -895,20 +893,20 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S5" s="8"/>
       <c r="V5" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -916,20 +914,20 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S6" s="8"/>
       <c r="V6" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -937,73 +935,73 @@
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S7" s="8"/>
       <c r="V7" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S8" s="8"/>
       <c r="V8" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S9" s="8"/>
       <c r="V9" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S10" s="8"/>
       <c r="V10" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -1015,17 +1013,17 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M11" s="7"/>
       <c r="S11" s="8"/>
       <c r="V11" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -1037,80 +1035,80 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S12" s="8"/>
       <c r="V12" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G13" s="7"/>
       <c r="I13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S13" s="8"/>
       <c r="V13" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="G14" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S14" s="8"/>
       <c r="V14" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="G15" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S15" s="8"/>
       <c r="V15" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
@@ -1119,19 +1117,19 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S16" s="8"/>
       <c r="V16" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1140,14 +1138,14 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S17" s="8"/>
       <c r="V17" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
@@ -1161,14 +1159,14 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S18" s="8"/>
       <c r="V18" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -1182,19 +1180,19 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S19" s="8"/>
       <c r="V19" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
@@ -1203,19 +1201,19 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S20" s="8"/>
       <c r="V20" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
@@ -1223,24 +1221,24 @@
       <c r="E21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S21" s="8"/>
       <c r="V21" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1248,25 +1246,25 @@
       <c r="H22" s="7"/>
       <c r="I22" s="8"/>
       <c r="J22" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S22" s="8"/>
       <c r="V22" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -1276,20 +1274,20 @@
       <c r="H23" s="7"/>
       <c r="I23" s="8"/>
       <c r="J23" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S23" s="8"/>
       <c r="V23" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1298,60 +1296,60 @@
       <c r="H24" s="7"/>
       <c r="I24" s="8"/>
       <c r="J24" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S24" s="8"/>
       <c r="V24" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="8"/>
       <c r="J25" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S25" s="8"/>
       <c r="V25" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="8"/>
       <c r="J26" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S26" s="8"/>
       <c r="V26" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
@@ -1359,21 +1357,21 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="8"/>
       <c r="J27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S27" s="8"/>
       <c r="V27" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
@@ -1382,23 +1380,23 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S28" s="8"/>
       <c r="V28" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1408,36 +1406,36 @@
       <c r="H29" s="7"/>
       <c r="I29" s="8"/>
       <c r="K29" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S29" s="8"/>
       <c r="V29" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="8"/>
       <c r="K30" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S30" s="8"/>
       <c r="V30" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -1451,20 +1449,20 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I31" s="8"/>
       <c r="K31" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S31" s="8"/>
       <c r="V31" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
@@ -1472,21 +1470,21 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="8"/>
       <c r="L32" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S32" s="8"/>
       <c r="V32" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
@@ -1495,86 +1493,86 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I33" s="8"/>
       <c r="L33" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S33" s="8"/>
       <c r="V33" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="8"/>
       <c r="M34" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S34" s="8"/>
       <c r="V34" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="8"/>
       <c r="M35" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S35" s="8"/>
       <c r="V35" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="8"/>
       <c r="M36" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S36" s="8"/>
       <c r="V36" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -1582,21 +1580,21 @@
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="8"/>
       <c r="M37" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S37" s="8"/>
       <c r="V37" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
@@ -1604,16 +1602,16 @@
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="8"/>
       <c r="M38" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S38" s="8"/>
       <c r="V38" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -1627,23 +1625,23 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I39" s="8"/>
       <c r="M39" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S39" s="8"/>
       <c r="V39" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -1653,19 +1651,19 @@
       <c r="H40" s="7"/>
       <c r="I40" s="8"/>
       <c r="N40" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S40" s="8"/>
       <c r="V40" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -1675,19 +1673,19 @@
       <c r="H41" s="7"/>
       <c r="I41" s="8"/>
       <c r="N41" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S41" s="8"/>
       <c r="V41" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -1697,20 +1695,20 @@
       <c r="H42" s="7"/>
       <c r="I42" s="8"/>
       <c r="N42" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S42" s="8"/>
       <c r="V42" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -1719,20 +1717,1572 @@
       <c r="H43" s="7"/>
       <c r="I43" s="8"/>
       <c r="N43" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S43" s="8"/>
       <c r="V43" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="8"/>
+      <c r="N44" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S44" s="8"/>
+      <c r="V44" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="8"/>
+      <c r="N45" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S45" s="8"/>
+      <c r="V45" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="8"/>
+      <c r="N46" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S46" s="8"/>
+      <c r="V46" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H47" s="7"/>
+      <c r="I47" s="8"/>
+      <c r="N47" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S47" s="8"/>
+      <c r="V47" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="8"/>
+      <c r="O48" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S48" s="8"/>
+      <c r="V48" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H49" s="7"/>
+      <c r="I49" s="8"/>
+      <c r="O49" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S49" s="8"/>
+      <c r="V49" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+      <c r="I50" s="8"/>
+      <c r="Q50" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R50" s="7"/>
+      <c r="S50" s="8"/>
+      <c r="V50" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="8"/>
+      <c r="Q51" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R51" s="7"/>
+      <c r="S51" s="8"/>
+      <c r="V51" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="8"/>
+      <c r="M52" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S52" s="8"/>
+      <c r="T52" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U52" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="8"/>
+      <c r="O53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S53" s="8"/>
+      <c r="T53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U53" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="8"/>
+      <c r="P54" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S54" s="8"/>
+      <c r="T54" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U54" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="8"/>
+      <c r="P55" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S55" s="8"/>
+      <c r="T55" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="8"/>
+      <c r="P56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S56" s="8"/>
+      <c r="T56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U56" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="8"/>
+      <c r="P57" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S57" s="8"/>
+      <c r="T57" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U57" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="8"/>
+      <c r="P58" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S58" s="8"/>
+      <c r="T58" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U58" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="8"/>
+      <c r="P59" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S59" s="8"/>
+      <c r="U59" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+      <c r="I60" s="8"/>
+      <c r="P60" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S60" s="8"/>
+      <c r="U60" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="8"/>
+      <c r="P61" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S61" s="8"/>
+      <c r="T61" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="8"/>
+      <c r="R62" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S62" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="8"/>
+      <c r="R63" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S63" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+      <c r="I64" s="8"/>
+      <c r="R64" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S64" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="8"/>
+      <c r="R65" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S65" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V65">
+    <sortCondition descending="1" ref="V3:V65"/>
+    <sortCondition descending="1" ref="U3:U65"/>
+    <sortCondition descending="1" ref="T3:T65"/>
+    <sortCondition descending="1" ref="S3:S65"/>
+    <sortCondition descending="1" ref="I3:I65"/>
+    <sortCondition descending="1" ref="J3:J65"/>
+    <sortCondition descending="1" ref="K3:K65"/>
+    <sortCondition descending="1" ref="L3:L65"/>
+    <sortCondition descending="1" ref="M3:M65"/>
+    <sortCondition descending="1" ref="N3:N65"/>
+    <sortCondition descending="1" ref="O3:O65"/>
+    <sortCondition descending="1" ref="P3:P65"/>
+    <sortCondition descending="1" ref="Q3:Q65"/>
+    <sortCondition ref="R3:R65"/>
+    <sortCondition descending="1" ref="B3:B65"/>
+    <sortCondition descending="1" ref="C3:C65"/>
+    <sortCondition descending="1" ref="D3:D65"/>
+    <sortCondition descending="1" ref="E3:E65"/>
+    <sortCondition descending="1" ref="F3:F65"/>
+    <sortCondition descending="1" ref="G3:G65"/>
+    <sortCondition descending="1" ref="H3:H65"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:Q1"/>
+    <mergeCell ref="S1:V1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B3DCEF-5D6A-B948-BE1C-1FE631050A9D}">
+  <dimension ref="A1:V65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="104.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.6640625" customWidth="1"/>
+    <col min="19" max="22" width="3.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+    </row>
+    <row r="2" spans="1:22" ht="102" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S3" s="8"/>
+      <c r="V3" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S4" s="8"/>
+      <c r="V4" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S5" s="8"/>
+      <c r="V5" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S6" s="8"/>
+      <c r="V6" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="8"/>
+      <c r="V7" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S8" s="8"/>
+      <c r="V8" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" s="8"/>
+      <c r="V9" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S10" s="8"/>
+      <c r="V10" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="S11" s="8"/>
+      <c r="V11" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S12" s="8"/>
+      <c r="V12" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="I13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S13" s="8"/>
+      <c r="V13" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="G14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S14" s="8"/>
+      <c r="V14" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>35</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S15" s="8"/>
+      <c r="V15" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S16" s="8"/>
+      <c r="V16" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S17" s="8"/>
+      <c r="V17" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S18" s="8"/>
+      <c r="V18" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S19" s="8"/>
+      <c r="V19" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S20" s="8"/>
+      <c r="V20" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S21" s="8"/>
+      <c r="V21" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S22" s="8"/>
+      <c r="V22" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S23" s="8"/>
+      <c r="V23" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S24" s="8"/>
+      <c r="V24" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S25" s="8"/>
+      <c r="V25" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S26" s="8"/>
+      <c r="V26" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S27" s="8"/>
+      <c r="V27" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="8"/>
+      <c r="J28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S28" s="8"/>
+      <c r="V28" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="8"/>
+      <c r="K29" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S29" s="8"/>
+      <c r="V29" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="8"/>
+      <c r="K30" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S30" s="8"/>
+      <c r="V30" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="K31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S31" s="8"/>
+      <c r="V31" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="8"/>
+      <c r="L32" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S32" s="8"/>
+      <c r="V32" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="8"/>
+      <c r="L33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S33" s="8"/>
+      <c r="V33" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="8"/>
+      <c r="M34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S34" s="8"/>
+      <c r="T34" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U34" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="8"/>
+      <c r="M35" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S35" s="8"/>
+      <c r="V35" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="8"/>
+      <c r="M36" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S36" s="8"/>
+      <c r="V36" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="8"/>
+      <c r="M37" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S37" s="8"/>
+      <c r="V37" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="8"/>
+      <c r="M38" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S38" s="8"/>
+      <c r="V38" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="7"/>
+      <c r="I39" s="8"/>
+      <c r="M39" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S39" s="8"/>
+      <c r="V39" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I40" s="8"/>
+      <c r="M40" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S40" s="8"/>
+      <c r="V40" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="8"/>
+      <c r="N41" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S41" s="8"/>
+      <c r="V41" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="8"/>
+      <c r="N42" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S42" s="8"/>
+      <c r="V42" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="8"/>
+      <c r="N43" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S43" s="8"/>
+      <c r="V43" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>43</v>
       </c>
       <c r="B44" s="6"/>
       <c r="C44" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -1741,11 +3291,11 @@
       <c r="H44" s="7"/>
       <c r="I44" s="8"/>
       <c r="N44" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S44" s="8"/>
       <c r="V44" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -1755,7 +3305,7 @@
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
@@ -1763,21 +3313,21 @@
       <c r="H45" s="7"/>
       <c r="I45" s="8"/>
       <c r="N45" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S45" s="8"/>
       <c r="V45" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -1785,38 +3335,38 @@
       <c r="H46" s="7"/>
       <c r="I46" s="8"/>
       <c r="N46" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S46" s="8"/>
       <c r="V46" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
       <c r="I47" s="8"/>
       <c r="N47" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S47" s="8"/>
       <c r="V47" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="7"/>
@@ -1824,24 +3374,24 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H48" s="7"/>
       <c r="I48" s="8"/>
       <c r="N48" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S48" s="8"/>
       <c r="V48" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -1851,87 +3401,91 @@
       <c r="H49" s="7"/>
       <c r="I49" s="8"/>
       <c r="O49" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S49" s="8"/>
       <c r="V49" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="6"/>
+      <c r="B50" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
-      <c r="G50" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="G50" s="7"/>
       <c r="H50" s="7"/>
       <c r="I50" s="8"/>
       <c r="O50" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S50" s="8"/>
-      <c r="V50" s="7" t="s">
-        <v>48</v>
+      <c r="T50" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U50" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>48</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B51" s="6"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
+      <c r="G51" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="H51" s="7"/>
       <c r="I51" s="8"/>
-      <c r="Q51" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R51" s="7"/>
+      <c r="O51" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="S51" s="8"/>
       <c r="V51" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="7" t="s">
-        <v>48</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
       <c r="I52" s="8"/>
-      <c r="Q52" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R52" s="7"/>
+      <c r="P52" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="S52" s="8"/>
-      <c r="V52" s="7" t="s">
-        <v>48</v>
+      <c r="T52" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="U52" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -1940,15 +3494,15 @@
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="8"/>
-      <c r="M53" s="7" t="s">
-        <v>48</v>
+      <c r="P53" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="S53" s="8"/>
       <c r="T53" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U53" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.2">
@@ -1956,7 +3510,7 @@
         <v>78</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
@@ -1965,25 +3519,22 @@
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
       <c r="I54" s="8"/>
-      <c r="O54" s="7" t="s">
-        <v>48</v>
+      <c r="P54" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="S54" s="8"/>
       <c r="T54" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="U54" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
@@ -1991,39 +3542,39 @@
       <c r="H55" s="7"/>
       <c r="I55" s="8"/>
       <c r="P55" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S55" s="8"/>
       <c r="T55" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U55" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>83</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>48</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B56" s="6"/>
       <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
+      <c r="D56" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="8"/>
       <c r="P56" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S56" s="8"/>
       <c r="T56" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U56" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
@@ -2031,125 +3582,121 @@
         <v>84</v>
       </c>
       <c r="B57" s="6"/>
-      <c r="C57" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="C57" s="7"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
+      <c r="E57" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
       <c r="H57" s="7"/>
       <c r="I57" s="8"/>
       <c r="P57" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S57" s="8"/>
-      <c r="T57" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="U57" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B58" s="6"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="D58" s="7"/>
       <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
+      <c r="F58" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="G58" s="7"/>
       <c r="H58" s="7"/>
       <c r="I58" s="8"/>
       <c r="P58" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S58" s="8"/>
       <c r="T58" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U58" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B59" s="6"/>
+      <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
       <c r="I59" s="8"/>
       <c r="P59" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S59" s="8"/>
-      <c r="T59" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="U59" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>46</v>
+      </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
-      <c r="E60" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="E60" s="7"/>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
       <c r="I60" s="8"/>
-      <c r="P60" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="Q60" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R60" s="7"/>
       <c r="S60" s="8"/>
-      <c r="U60" s="7" t="s">
-        <v>48</v>
+      <c r="V60" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B61" s="6"/>
-      <c r="C61" s="7"/>
+      <c r="C61" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
-      <c r="F61" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="F61" s="7"/>
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
       <c r="I61" s="8"/>
-      <c r="P61" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="Q61" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R61" s="7"/>
       <c r="S61" s="8"/>
-      <c r="U61" s="7" t="s">
-        <v>48</v>
+      <c r="V61" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -2158,43 +3705,42 @@
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
       <c r="I62" s="8"/>
-      <c r="P62" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S62" s="8"/>
-      <c r="T62" s="7" t="s">
-        <v>48</v>
+      <c r="R62" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S62" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>89</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>48</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B63" s="6"/>
       <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
+      <c r="D63" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
       <c r="H63" s="7"/>
       <c r="I63" s="8"/>
       <c r="R63" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S63" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B64" s="6"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
@@ -2202,77 +3748,56 @@
       <c r="H64" s="7"/>
       <c r="I64" s="8"/>
       <c r="R64" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S64" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B65" s="6"/>
       <c r="C65" s="7"/>
-      <c r="D65" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="D65" s="7"/>
       <c r="E65" s="7"/>
-      <c r="F65" s="7"/>
+      <c r="F65" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
       <c r="I65" s="8"/>
       <c r="R65" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S65" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>15</v>
-      </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7"/>
-      <c r="F66" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7"/>
-      <c r="I66" s="8"/>
-      <c r="R66" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S66" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V66">
-    <sortCondition descending="1" ref="V3:V66"/>
-    <sortCondition descending="1" ref="U3:U66"/>
-    <sortCondition descending="1" ref="T3:T66"/>
-    <sortCondition descending="1" ref="S3:S66"/>
-    <sortCondition descending="1" ref="I3:I66"/>
-    <sortCondition descending="1" ref="J3:J66"/>
-    <sortCondition descending="1" ref="K3:K66"/>
-    <sortCondition descending="1" ref="L3:L66"/>
-    <sortCondition descending="1" ref="M3:M66"/>
-    <sortCondition descending="1" ref="N3:N66"/>
-    <sortCondition descending="1" ref="O3:O66"/>
-    <sortCondition descending="1" ref="P3:P66"/>
-    <sortCondition descending="1" ref="Q3:Q66"/>
-    <sortCondition ref="R3:R66"/>
-    <sortCondition descending="1" ref="B3:B66"/>
-    <sortCondition descending="1" ref="C3:C66"/>
-    <sortCondition descending="1" ref="D3:D66"/>
-    <sortCondition descending="1" ref="E3:E66"/>
-    <sortCondition descending="1" ref="F3:F66"/>
-    <sortCondition descending="1" ref="G3:G66"/>
-    <sortCondition descending="1" ref="H3:H66"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:V65">
+    <sortCondition descending="1" ref="I3:I65"/>
+    <sortCondition descending="1" ref="J3:J65"/>
+    <sortCondition descending="1" ref="K3:K65"/>
+    <sortCondition descending="1" ref="L3:L65"/>
+    <sortCondition descending="1" ref="M3:M65"/>
+    <sortCondition descending="1" ref="N3:N65"/>
+    <sortCondition descending="1" ref="O3:O65"/>
+    <sortCondition descending="1" ref="P3:P65"/>
+    <sortCondition descending="1" ref="Q3:Q65"/>
+    <sortCondition descending="1" ref="R3:R65"/>
+    <sortCondition descending="1" ref="B3:B65"/>
+    <sortCondition descending="1" ref="C3:C65"/>
+    <sortCondition descending="1" ref="D3:D65"/>
+    <sortCondition descending="1" ref="E3:E65"/>
+    <sortCondition descending="1" ref="F3:F65"/>
+    <sortCondition descending="1" ref="G3:G65"/>
+    <sortCondition descending="1" ref="H3:H65"/>
+    <sortCondition descending="1" ref="V3:V65"/>
+    <sortCondition descending="1" ref="U3:U65"/>
+    <sortCondition descending="1" ref="T3:T65"/>
+    <sortCondition descending="1" ref="S3:S65"/>
   </sortState>
   <mergeCells count="3">
     <mergeCell ref="B1:H1"/>

</xml_diff>